<commit_message>
Release 1.23 compiles, unit tests passed.
</commit_message>
<xml_diff>
--- a/package/kutils/inst/extdata/natlongsurv.templ.xlsx
+++ b/package/kutils/inst/extdata/natlongsurv.templ.xlsx
@@ -3,213 +3,178 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="key" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="varlab" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
-  <si>
-    <t>name_old</t>
-  </si>
-  <si>
-    <t>name_new</t>
-  </si>
-  <si>
-    <t>class_old</t>
-  </si>
-  <si>
-    <t>class_new</t>
-  </si>
-  <si>
-    <t>value_old</t>
-  </si>
-  <si>
-    <t>value_new</t>
-  </si>
-  <si>
-    <t>missings</t>
-  </si>
-  <si>
-    <t>recodes</t>
-  </si>
-  <si>
-    <t>R0000100</t>
-  </si>
-  <si>
-    <t>integer</t>
-  </si>
-  <si>
-    <t>1|2|3|4|5|6|7|8|9|10|11|12|13|14|15</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>R0003300</t>
-  </si>
-  <si>
-    <t>1|2|3|4|5|6</t>
-  </si>
-  <si>
-    <t>R0005700</t>
-  </si>
-  <si>
-    <t>-4|11|12|13|14|15|16|17|18|19|20|21|22|23|24</t>
-  </si>
-  <si>
-    <t>R0060300</t>
-  </si>
-  <si>
-    <t>-4|72|82|91|98|99|103|110|111|112|113|114|121|125|129</t>
-  </si>
-  <si>
-    <t>R1051600</t>
-  </si>
-  <si>
-    <t>-5|-4|9|10|11|12|13|14|15|16|17|18</t>
-  </si>
-  <si>
-    <t>R1302000</t>
-  </si>
-  <si>
-    <t>-5|-4|0|1</t>
-  </si>
-  <si>
-    <t>R1302100</t>
-  </si>
-  <si>
-    <t>-5|-4|1|4|5|6|7|8|10|12|15|18|20|25|30</t>
-  </si>
-  <si>
-    <t>R1303400</t>
-  </si>
-  <si>
-    <t>-5|-4|-1|1|2|3|4|5|6|8|10|11|20|28|30</t>
-  </si>
-  <si>
-    <t>R6235600</t>
-  </si>
-  <si>
-    <t>-5|0|6|7|8|9|10|11|12|13|14|15|16|17|18</t>
-  </si>
-  <si>
-    <t>R6502300</t>
-  </si>
-  <si>
-    <t>-4|1|3|4|9|14</t>
-  </si>
-  <si>
-    <t>R6513700</t>
-  </si>
-  <si>
-    <t>-5|49|50|51|52|53|54|55|56|57|58|59|60|61|80</t>
-  </si>
-  <si>
-    <t>R6516200</t>
-  </si>
-  <si>
-    <t>-5|1|3|4|5|6</t>
-  </si>
-  <si>
-    <t>R6520300</t>
-  </si>
-  <si>
-    <t>-5|-4|-2|-1|1|2|3|4|5|6|7|8|9|10|11</t>
-  </si>
-  <si>
-    <t>R6553600</t>
-  </si>
-  <si>
-    <t>-5|-4|-2|-1|4|5|6|7|8|11</t>
-  </si>
-  <si>
-    <t>R7289200</t>
-  </si>
-  <si>
-    <t>-5|-4|-2|-1|0|1</t>
-  </si>
-  <si>
-    <t>R7289400</t>
-  </si>
-  <si>
-    <t>-5|-4|-2|0|1</t>
-  </si>
-  <si>
-    <t>R7293430</t>
-  </si>
-  <si>
-    <t>-5|373|406|417|427|465|517|530|537|538|553|560|584|626|637</t>
-  </si>
-  <si>
-    <t>R7312300</t>
-  </si>
-  <si>
-    <t>-5|-4|-2|-1|5000|7000|16000|18000|25000|35000|52000|53000|59800|64000|105000</t>
-  </si>
-  <si>
-    <t>R7329900</t>
-  </si>
-  <si>
-    <t>-5|-4|-2|-1|1|2|3|4|5|6|7</t>
-  </si>
-  <si>
-    <t>R7330000</t>
-  </si>
-  <si>
-    <t>-5|-2|-1|20000|22000|25000|30000|35000|36000|50000|53000|60000|65000|90000|100000</t>
-  </si>
-  <si>
-    <t>R7337600</t>
-  </si>
-  <si>
-    <t>R7344600</t>
-  </si>
-  <si>
-    <t>-5|-4|-2|-1|1|2|3|4</t>
-  </si>
-  <si>
-    <t>R7344700</t>
-  </si>
-  <si>
-    <t>R7347500</t>
-  </si>
-  <si>
-    <t>-5|-2|-1|0|200|1000|2000|2500|3000|3300|3500|5000|6000|7000|10000</t>
-  </si>
-  <si>
-    <t>R7347600</t>
-  </si>
-  <si>
-    <t>-5|-4|-2|-1|0|200|500|1000|1500|2500|3000|3300|3500|5000|10000</t>
-  </si>
-  <si>
-    <t>R7347700</t>
-  </si>
-  <si>
-    <t>-5|-4|-2|-1|0|100|1500|2000|2500|3000|3400|4000|5000|7500|10000</t>
-  </si>
-  <si>
-    <t>R7477700</t>
-  </si>
-  <si>
-    <t>-5|-4|0|1|2|3|4|5|6|7|8|9|10|12|15</t>
-  </si>
-  <si>
-    <t>R7477800</t>
-  </si>
-  <si>
-    <t>-5|-4|0|1|2|3|4|5|7</t>
-  </si>
-  <si>
-    <t>R7610300</t>
-  </si>
-  <si>
-    <t>-5|0|1|9</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+  <si>
+    <t xml:space="preserve">name_old</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name_new</t>
+  </si>
+  <si>
+    <t xml:space="preserve">class_old</t>
+  </si>
+  <si>
+    <t xml:space="preserve">class_new</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_old</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value_new</t>
+  </si>
+  <si>
+    <t xml:space="preserve">missings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">recodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R0000100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">R0003300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1|2|3|4|5|6|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R0005700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R0060300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1051600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5|-4|9|10|11|12|13|14|15|16|17|18|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1302000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5|-4|0|1|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1302100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R1303400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6235600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6502300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4|1|3|14|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6513700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6516200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5|1|3|4|5|6|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6520300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5|-4|-2|-1|1|2|3|4|5|6|7|8|9|10|11|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R6553600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5|-4|-2|-1|4|5|6|7|8|11|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7289200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5|-4|-2|-1|0|1|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7289400</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5|-4|-2|0|1|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7293430</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7312300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7329900</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5|-4|-2|-1|1|2|3|4|5|6|7|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7330000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7337600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7344600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5|-4|-2|-1|1|2|3|4|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7344700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7347500</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7347600</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7347700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7477700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7477800</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5|-4|0|1|2|3|4|5|7|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7610300</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5|0|1|9|.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">varlab</t>
   </si>
 </sst>
 </file>
@@ -254,6 +219,34 @@
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H30" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:H30"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="name_old"/>
+    <tableColumn id="2" name="name_new"/>
+    <tableColumn id="3" name="class_old"/>
+    <tableColumn id="4" name="class_new"/>
+    <tableColumn id="5" name="value_old"/>
+    <tableColumn id="6" name="value_new"/>
+    <tableColumn id="7" name="missings"/>
+    <tableColumn id="8" name="recodes"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A1:B30" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:B30"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="name_new"/>
+    <tableColumn id="2" name="varlab"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -534,7 +527,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
@@ -633,10 +626,10 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -647,10 +640,10 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
@@ -659,10 +652,10 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -673,10 +666,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -685,10 +678,10 @@
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -699,10 +692,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -711,10 +704,10 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -725,10 +718,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -737,10 +730,10 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -751,10 +744,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -763,10 +756,10 @@
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
@@ -777,10 +770,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -789,10 +782,10 @@
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
@@ -803,10 +796,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -815,10 +808,10 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -829,10 +822,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -841,10 +834,10 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -855,10 +848,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -867,10 +860,10 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
@@ -881,10 +874,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -893,10 +886,10 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -907,10 +900,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -919,10 +912,10 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
@@ -933,10 +926,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -945,10 +938,10 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
@@ -959,10 +952,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -971,10 +964,10 @@
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G17" t="s">
         <v>11</v>
@@ -985,10 +978,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -997,10 +990,10 @@
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="G18" t="s">
         <v>11</v>
@@ -1011,10 +1004,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -1023,10 +1016,10 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
@@ -1037,10 +1030,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="B20" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -1049,10 +1042,10 @@
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F20" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="G20" t="s">
         <v>11</v>
@@ -1063,10 +1056,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -1075,10 +1068,10 @@
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="G21" t="s">
         <v>11</v>
@@ -1089,10 +1082,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B22" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -1101,10 +1094,10 @@
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G22" t="s">
         <v>11</v>
@@ -1115,10 +1108,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -1127,10 +1120,10 @@
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F23" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="G23" t="s">
         <v>11</v>
@@ -1141,10 +1134,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -1153,10 +1146,10 @@
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F24" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="G24" t="s">
         <v>11</v>
@@ -1167,10 +1160,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -1179,10 +1172,10 @@
         <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>55</v>
+        <v>10</v>
       </c>
       <c r="G25" t="s">
         <v>11</v>
@@ -1193,10 +1186,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -1205,10 +1198,10 @@
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="G26" t="s">
         <v>11</v>
@@ -1219,10 +1212,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -1231,10 +1224,10 @@
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="G27" t="s">
         <v>11</v>
@@ -1245,10 +1238,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -1257,10 +1250,10 @@
         <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="G28" t="s">
         <v>11</v>
@@ -1271,10 +1264,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -1283,10 +1276,10 @@
         <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="G29" t="s">
         <v>11</v>
@@ -1297,10 +1290,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="C30" t="s">
         <v>9</v>
@@ -1309,10 +1302,10 @@
         <v>9</v>
       </c>
       <c r="E30" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="F30" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="G30" t="s">
         <v>11</v>
@@ -1324,5 +1317,265 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+      <c r="B29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
variableKey: finally solved issues with unit tests.  Treatment of factors solved.
</commit_message>
<xml_diff>
--- a/package/kutils/inst/extdata/natlongsurv.templ.xlsx
+++ b/package/kutils/inst/extdata/natlongsurv.templ.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t xml:space="preserve">name_old</t>
   </si>
@@ -54,7 +54,22 @@
     <t xml:space="preserve">R0003300</t>
   </si>
   <si>
-    <t xml:space="preserve">1|2|3|4|5|6|.</t>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6</t>
   </si>
   <si>
     <t xml:space="preserve">R0005700</t>
@@ -66,13 +81,46 @@
     <t xml:space="preserve">R1051600</t>
   </si>
   <si>
-    <t xml:space="preserve">-5|-4|9|10|11|12|13|14|15|16|17|18|.</t>
+    <t xml:space="preserve">-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
   </si>
   <si>
     <t xml:space="preserve">R1302000</t>
   </si>
   <si>
-    <t xml:space="preserve">-5|-4|0|1|.</t>
+    <t xml:space="preserve">0</t>
   </si>
   <si>
     <t xml:space="preserve">R1302100</t>
@@ -87,42 +135,36 @@
     <t xml:space="preserve">R6502300</t>
   </si>
   <si>
-    <t xml:space="preserve">-4|1|3|14|.</t>
-  </si>
-  <si>
     <t xml:space="preserve">R6513700</t>
   </si>
   <si>
     <t xml:space="preserve">R6516200</t>
   </si>
   <si>
-    <t xml:space="preserve">-5|1|3|4|5|6|.</t>
-  </si>
-  <si>
     <t xml:space="preserve">R6520300</t>
   </si>
   <si>
-    <t xml:space="preserve">-5|-4|-2|-1|1|2|3|4|5|6|7|8|9|10|11|.</t>
+    <t xml:space="preserve">-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8</t>
   </si>
   <si>
     <t xml:space="preserve">R6553600</t>
   </si>
   <si>
-    <t xml:space="preserve">-5|-4|-2|-1|4|5|6|7|8|11|.</t>
-  </si>
-  <si>
     <t xml:space="preserve">R7289200</t>
   </si>
   <si>
-    <t xml:space="preserve">-5|-4|-2|-1|0|1|.</t>
-  </si>
-  <si>
     <t xml:space="preserve">R7289400</t>
   </si>
   <si>
-    <t xml:space="preserve">-5|-4|-2|0|1|.</t>
-  </si>
-  <si>
     <t xml:space="preserve">R7293430</t>
   </si>
   <si>
@@ -132,9 +174,6 @@
     <t xml:space="preserve">R7329900</t>
   </si>
   <si>
-    <t xml:space="preserve">-5|-4|-2|-1|1|2|3|4|5|6|7|.</t>
-  </si>
-  <si>
     <t xml:space="preserve">R7330000</t>
   </si>
   <si>
@@ -144,9 +183,6 @@
     <t xml:space="preserve">R7344600</t>
   </si>
   <si>
-    <t xml:space="preserve">-5|-4|-2|-1|1|2|3|4|.</t>
-  </si>
-  <si>
     <t xml:space="preserve">R7344700</t>
   </si>
   <si>
@@ -165,13 +201,7 @@
     <t xml:space="preserve">R7477800</t>
   </si>
   <si>
-    <t xml:space="preserve">-5|-4|0|1|2|3|4|5|7|.</t>
-  </si>
-  <si>
     <t xml:space="preserve">R7610300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">-5|0|1|9|.</t>
   </si>
   <si>
     <t xml:space="preserve">varlab</t>
@@ -222,8 +252,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H30" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:H30"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:H140" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:H140"/>
   <tableColumns count="8">
     <tableColumn id="1" name="name_old"/>
     <tableColumn id="2" name="name_new"/>
@@ -614,22 +644,22 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -640,22 +670,22 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" t="s">
+      <c r="F5" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
       </c>
       <c r="G5" t="s">
         <v>11</v>
@@ -666,22 +696,22 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="F6" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -692,10 +722,10 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -704,10 +734,10 @@
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -718,10 +748,10 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -730,10 +760,10 @@
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
@@ -744,10 +774,10 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>9</v>
@@ -770,10 +800,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
@@ -796,10 +826,10 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
         <v>9</v>
@@ -808,10 +838,10 @@
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
@@ -822,10 +852,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
@@ -834,10 +864,10 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
@@ -848,10 +878,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C13" t="s">
         <v>9</v>
@@ -860,10 +890,10 @@
         <v>9</v>
       </c>
       <c r="E13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
@@ -874,10 +904,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
@@ -886,10 +916,10 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="G14" t="s">
         <v>11</v>
@@ -900,10 +930,10 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
@@ -912,10 +942,10 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
@@ -926,10 +956,10 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
@@ -938,10 +968,10 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="G16" t="s">
         <v>11</v>
@@ -952,10 +982,10 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
@@ -964,10 +994,10 @@
         <v>9</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F17" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="G17" t="s">
         <v>11</v>
@@ -978,10 +1008,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
@@ -990,10 +1020,10 @@
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="F18" t="s">
-        <v>10</v>
+        <v>28</v>
       </c>
       <c r="G18" t="s">
         <v>11</v>
@@ -1004,10 +1034,10 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C19" t="s">
         <v>9</v>
@@ -1016,10 +1046,10 @@
         <v>9</v>
       </c>
       <c r="E19" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
@@ -1030,10 +1060,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C20" t="s">
         <v>9</v>
@@ -1042,10 +1072,10 @@
         <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F20" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="G20" t="s">
         <v>11</v>
@@ -1056,10 +1086,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>9</v>
@@ -1068,10 +1098,10 @@
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="F21" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="G21" t="s">
         <v>11</v>
@@ -1082,10 +1112,10 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
         <v>9</v>
@@ -1094,10 +1124,10 @@
         <v>9</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="G22" t="s">
         <v>11</v>
@@ -1108,10 +1138,10 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
@@ -1120,10 +1150,10 @@
         <v>9</v>
       </c>
       <c r="E23" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="F23" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="G23" t="s">
         <v>11</v>
@@ -1134,10 +1164,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C24" t="s">
         <v>9</v>
@@ -1146,10 +1176,10 @@
         <v>9</v>
       </c>
       <c r="E24" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>33</v>
+        <v>10</v>
       </c>
       <c r="G24" t="s">
         <v>11</v>
@@ -1160,10 +1190,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="C25" t="s">
         <v>9</v>
@@ -1172,10 +1202,10 @@
         <v>9</v>
       </c>
       <c r="E25" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="F25" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="G25" t="s">
         <v>11</v>
@@ -1186,10 +1216,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C26" t="s">
         <v>9</v>
@@ -1198,10 +1228,10 @@
         <v>9</v>
       </c>
       <c r="E26" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="F26" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="G26" t="s">
         <v>11</v>
@@ -1212,10 +1242,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C27" t="s">
         <v>9</v>
@@ -1224,10 +1254,10 @@
         <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="F27" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="G27" t="s">
         <v>11</v>
@@ -1238,10 +1268,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
         <v>9</v>
@@ -1250,10 +1280,10 @@
         <v>9</v>
       </c>
       <c r="E28" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F28" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G28" t="s">
         <v>11</v>
@@ -1264,10 +1294,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
         <v>9</v>
@@ -1276,10 +1306,10 @@
         <v>9</v>
       </c>
       <c r="E29" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="G29" t="s">
         <v>11</v>
@@ -1290,27 +1320,2887 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" t="s">
+        <v>10</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" t="s">
+        <v>10</v>
+      </c>
+      <c r="F31" t="s">
+        <v>10</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E32" t="s">
+        <v>10</v>
+      </c>
+      <c r="F32" t="s">
+        <v>10</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>23</v>
+      </c>
+      <c r="F33" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>13</v>
+      </c>
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F35" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>9</v>
+      </c>
+      <c r="E36" t="s">
+        <v>29</v>
+      </c>
+      <c r="F36" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
+        <v>9</v>
+      </c>
+      <c r="E37" t="s">
+        <v>10</v>
+      </c>
+      <c r="F37" t="s">
+        <v>10</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" t="s">
+        <v>10</v>
+      </c>
+      <c r="F38" t="s">
+        <v>10</v>
+      </c>
+      <c r="G38" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>41</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" t="s">
+        <v>22</v>
+      </c>
+      <c r="F39" t="s">
+        <v>22</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" t="s">
+        <v>13</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+      <c r="F41" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>41</v>
+      </c>
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" t="s">
+        <v>16</v>
+      </c>
+      <c r="F42" t="s">
+        <v>16</v>
+      </c>
+      <c r="G42" t="s">
+        <v>11</v>
+      </c>
+      <c r="H42" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" t="s">
+        <v>9</v>
+      </c>
+      <c r="E43" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" t="s">
+        <v>17</v>
+      </c>
+      <c r="G43" t="s">
+        <v>11</v>
+      </c>
+      <c r="H43" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" t="s">
+        <v>18</v>
+      </c>
+      <c r="G44" t="s">
+        <v>11</v>
+      </c>
+      <c r="H44" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s">
+        <v>9</v>
+      </c>
+      <c r="E45" t="s">
+        <v>10</v>
+      </c>
+      <c r="F45" t="s">
+        <v>10</v>
+      </c>
+      <c r="G45" t="s">
+        <v>11</v>
+      </c>
+      <c r="H45" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" t="s">
+        <v>42</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" t="s">
+        <v>42</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" t="s">
+        <v>23</v>
+      </c>
+      <c r="F47" t="s">
+        <v>23</v>
+      </c>
+      <c r="G47" t="s">
+        <v>11</v>
+      </c>
+      <c r="H47" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" t="s">
+        <v>42</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
+        <v>9</v>
+      </c>
+      <c r="E48" t="s">
+        <v>43</v>
+      </c>
+      <c r="F48" t="s">
+        <v>43</v>
+      </c>
+      <c r="G48" t="s">
+        <v>11</v>
+      </c>
+      <c r="H48" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" t="s">
+        <v>42</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>44</v>
+      </c>
+      <c r="F49" t="s">
+        <v>44</v>
+      </c>
+      <c r="G49" t="s">
+        <v>11</v>
+      </c>
+      <c r="H49" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" t="s">
+        <v>42</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s">
+        <v>9</v>
+      </c>
+      <c r="E50" t="s">
+        <v>13</v>
+      </c>
+      <c r="F50" t="s">
+        <v>13</v>
+      </c>
+      <c r="G50" t="s">
+        <v>11</v>
+      </c>
+      <c r="H50" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" t="s">
+        <v>42</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F51" t="s">
+        <v>14</v>
+      </c>
+      <c r="G51" t="s">
+        <v>11</v>
+      </c>
+      <c r="H51" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" t="s">
+        <v>42</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" t="s">
+        <v>9</v>
+      </c>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="F52" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52" t="s">
+        <v>11</v>
+      </c>
+      <c r="H52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H53" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" t="s">
+        <v>17</v>
+      </c>
+      <c r="F54" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54" t="s">
+        <v>11</v>
+      </c>
+      <c r="H54" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" t="s">
+        <v>18</v>
+      </c>
+      <c r="F55" t="s">
+        <v>18</v>
+      </c>
+      <c r="G55" t="s">
+        <v>11</v>
+      </c>
+      <c r="H55" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" t="s">
+        <v>42</v>
+      </c>
+      <c r="C56" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" t="s">
+        <v>45</v>
+      </c>
+      <c r="F56" t="s">
+        <v>45</v>
+      </c>
+      <c r="G56" t="s">
+        <v>11</v>
+      </c>
+      <c r="H56" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" t="s">
+        <v>42</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" t="s">
+        <v>46</v>
+      </c>
+      <c r="F57" t="s">
+        <v>46</v>
+      </c>
+      <c r="G57" t="s">
+        <v>11</v>
+      </c>
+      <c r="H57" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" t="s">
+        <v>42</v>
+      </c>
+      <c r="C58" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" t="s">
+        <v>9</v>
+      </c>
+      <c r="E58" t="s">
+        <v>24</v>
+      </c>
+      <c r="F58" t="s">
+        <v>24</v>
+      </c>
+      <c r="G58" t="s">
+        <v>11</v>
+      </c>
+      <c r="H58" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" t="s">
+        <v>42</v>
+      </c>
+      <c r="C59" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" t="s">
+        <v>9</v>
+      </c>
+      <c r="E59" t="s">
+        <v>25</v>
+      </c>
+      <c r="F59" t="s">
+        <v>25</v>
+      </c>
+      <c r="G59" t="s">
+        <v>11</v>
+      </c>
+      <c r="H59" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" t="s">
+        <v>42</v>
+      </c>
+      <c r="C60" t="s">
+        <v>9</v>
+      </c>
+      <c r="D60" t="s">
+        <v>9</v>
+      </c>
+      <c r="E60" t="s">
+        <v>26</v>
+      </c>
+      <c r="F60" t="s">
+        <v>26</v>
+      </c>
+      <c r="G60" t="s">
+        <v>11</v>
+      </c>
+      <c r="H60" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" t="s">
+        <v>42</v>
+      </c>
+      <c r="C61" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" t="s">
+        <v>9</v>
+      </c>
+      <c r="E61" t="s">
+        <v>10</v>
+      </c>
+      <c r="F61" t="s">
+        <v>10</v>
+      </c>
+      <c r="G61" t="s">
+        <v>11</v>
+      </c>
+      <c r="H61" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
+      </c>
+      <c r="D62" t="s">
+        <v>9</v>
+      </c>
+      <c r="E62" t="s">
+        <v>22</v>
+      </c>
+      <c r="F62" t="s">
+        <v>22</v>
+      </c>
+      <c r="G62" t="s">
+        <v>11</v>
+      </c>
+      <c r="H62" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>47</v>
+      </c>
+      <c r="B63" t="s">
+        <v>47</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
+      </c>
+      <c r="D63" t="s">
+        <v>9</v>
+      </c>
+      <c r="E63" t="s">
+        <v>23</v>
+      </c>
+      <c r="F63" t="s">
+        <v>23</v>
+      </c>
+      <c r="G63" t="s">
+        <v>11</v>
+      </c>
+      <c r="H63" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>47</v>
+      </c>
+      <c r="B64" t="s">
+        <v>47</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+      <c r="D64" t="s">
+        <v>9</v>
+      </c>
+      <c r="E64" t="s">
+        <v>43</v>
+      </c>
+      <c r="F64" t="s">
+        <v>43</v>
+      </c>
+      <c r="G64" t="s">
+        <v>11</v>
+      </c>
+      <c r="H64" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>47</v>
+      </c>
+      <c r="B65" t="s">
+        <v>47</v>
+      </c>
+      <c r="C65" t="s">
+        <v>9</v>
+      </c>
+      <c r="D65" t="s">
+        <v>9</v>
+      </c>
+      <c r="E65" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" t="s">
+        <v>44</v>
+      </c>
+      <c r="G65" t="s">
+        <v>11</v>
+      </c>
+      <c r="H65" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>47</v>
+      </c>
+      <c r="B66" t="s">
+        <v>47</v>
+      </c>
+      <c r="C66" t="s">
+        <v>9</v>
+      </c>
+      <c r="D66" t="s">
+        <v>9</v>
+      </c>
+      <c r="E66" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" t="s">
+        <v>16</v>
+      </c>
+      <c r="G66" t="s">
+        <v>11</v>
+      </c>
+      <c r="H66" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>47</v>
+      </c>
+      <c r="B67" t="s">
+        <v>47</v>
+      </c>
+      <c r="C67" t="s">
+        <v>9</v>
+      </c>
+      <c r="D67" t="s">
+        <v>9</v>
+      </c>
+      <c r="E67" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" t="s">
+        <v>17</v>
+      </c>
+      <c r="G67" t="s">
+        <v>11</v>
+      </c>
+      <c r="H67" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>47</v>
+      </c>
+      <c r="B68" t="s">
+        <v>47</v>
+      </c>
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+      <c r="D68" t="s">
+        <v>9</v>
+      </c>
+      <c r="E68" t="s">
+        <v>18</v>
+      </c>
+      <c r="F68" t="s">
+        <v>18</v>
+      </c>
+      <c r="G68" t="s">
+        <v>11</v>
+      </c>
+      <c r="H68" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>47</v>
+      </c>
+      <c r="B69" t="s">
+        <v>47</v>
+      </c>
+      <c r="C69" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" t="s">
+        <v>9</v>
+      </c>
+      <c r="E69" t="s">
+        <v>45</v>
+      </c>
+      <c r="F69" t="s">
+        <v>45</v>
+      </c>
+      <c r="G69" t="s">
+        <v>11</v>
+      </c>
+      <c r="H69" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>47</v>
+      </c>
+      <c r="B70" t="s">
+        <v>47</v>
+      </c>
+      <c r="C70" t="s">
+        <v>9</v>
+      </c>
+      <c r="D70" t="s">
+        <v>9</v>
+      </c>
+      <c r="E70" t="s">
+        <v>46</v>
+      </c>
+      <c r="F70" t="s">
+        <v>46</v>
+      </c>
+      <c r="G70" t="s">
+        <v>11</v>
+      </c>
+      <c r="H70" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>47</v>
+      </c>
+      <c r="B71" t="s">
+        <v>47</v>
+      </c>
+      <c r="C71" t="s">
+        <v>9</v>
+      </c>
+      <c r="D71" t="s">
+        <v>9</v>
+      </c>
+      <c r="E71" t="s">
+        <v>26</v>
+      </c>
+      <c r="F71" t="s">
+        <v>26</v>
+      </c>
+      <c r="G71" t="s">
+        <v>11</v>
+      </c>
+      <c r="H71" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>47</v>
+      </c>
+      <c r="B72" t="s">
+        <v>47</v>
+      </c>
+      <c r="C72" t="s">
+        <v>9</v>
+      </c>
+      <c r="D72" t="s">
+        <v>9</v>
+      </c>
+      <c r="E72" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" t="s">
+        <v>10</v>
+      </c>
+      <c r="G72" t="s">
+        <v>11</v>
+      </c>
+      <c r="H72" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>48</v>
+      </c>
+      <c r="B73" t="s">
+        <v>48</v>
+      </c>
+      <c r="C73" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73" t="s">
+        <v>9</v>
+      </c>
+      <c r="E73" t="s">
+        <v>22</v>
+      </c>
+      <c r="F73" t="s">
+        <v>22</v>
+      </c>
+      <c r="G73" t="s">
+        <v>11</v>
+      </c>
+      <c r="H73" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>48</v>
+      </c>
+      <c r="B74" t="s">
+        <v>48</v>
+      </c>
+      <c r="C74" t="s">
+        <v>9</v>
+      </c>
+      <c r="D74" t="s">
+        <v>9</v>
+      </c>
+      <c r="E74" t="s">
+        <v>23</v>
+      </c>
+      <c r="F74" t="s">
+        <v>23</v>
+      </c>
+      <c r="G74" t="s">
+        <v>11</v>
+      </c>
+      <c r="H74" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>48</v>
+      </c>
+      <c r="B75" t="s">
+        <v>48</v>
+      </c>
+      <c r="C75" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" t="s">
+        <v>9</v>
+      </c>
+      <c r="E75" t="s">
+        <v>43</v>
+      </c>
+      <c r="F75" t="s">
+        <v>43</v>
+      </c>
+      <c r="G75" t="s">
+        <v>11</v>
+      </c>
+      <c r="H75" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>48</v>
+      </c>
+      <c r="B76" t="s">
+        <v>48</v>
+      </c>
+      <c r="C76" t="s">
+        <v>9</v>
+      </c>
+      <c r="D76" t="s">
+        <v>9</v>
+      </c>
+      <c r="E76" t="s">
+        <v>44</v>
+      </c>
+      <c r="F76" t="s">
+        <v>44</v>
+      </c>
+      <c r="G76" t="s">
+        <v>11</v>
+      </c>
+      <c r="H76" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>48</v>
+      </c>
+      <c r="B77" t="s">
+        <v>48</v>
+      </c>
+      <c r="C77" t="s">
+        <v>9</v>
+      </c>
+      <c r="D77" t="s">
+        <v>9</v>
+      </c>
+      <c r="E77" t="s">
+        <v>35</v>
+      </c>
+      <c r="F77" t="s">
+        <v>35</v>
+      </c>
+      <c r="G77" t="s">
+        <v>11</v>
+      </c>
+      <c r="H77" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>48</v>
+      </c>
+      <c r="B78" t="s">
+        <v>48</v>
+      </c>
+      <c r="C78" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78" t="s">
+        <v>9</v>
+      </c>
+      <c r="E78" t="s">
+        <v>13</v>
+      </c>
+      <c r="F78" t="s">
+        <v>13</v>
+      </c>
+      <c r="G78" t="s">
+        <v>11</v>
+      </c>
+      <c r="H78" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>48</v>
+      </c>
+      <c r="B79" t="s">
+        <v>48</v>
+      </c>
+      <c r="C79" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" t="s">
+        <v>9</v>
+      </c>
+      <c r="E79" t="s">
+        <v>10</v>
+      </c>
+      <c r="F79" t="s">
+        <v>10</v>
+      </c>
+      <c r="G79" t="s">
+        <v>11</v>
+      </c>
+      <c r="H79" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="s">
+        <v>49</v>
+      </c>
+      <c r="B80" t="s">
+        <v>49</v>
+      </c>
+      <c r="C80" t="s">
+        <v>9</v>
+      </c>
+      <c r="D80" t="s">
+        <v>9</v>
+      </c>
+      <c r="E80" t="s">
+        <v>22</v>
+      </c>
+      <c r="F80" t="s">
+        <v>22</v>
+      </c>
+      <c r="G80" t="s">
+        <v>11</v>
+      </c>
+      <c r="H80" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="s">
+        <v>49</v>
+      </c>
+      <c r="B81" t="s">
+        <v>49</v>
+      </c>
+      <c r="C81" t="s">
+        <v>9</v>
+      </c>
+      <c r="D81" t="s">
+        <v>9</v>
+      </c>
+      <c r="E81" t="s">
+        <v>23</v>
+      </c>
+      <c r="F81" t="s">
+        <v>23</v>
+      </c>
+      <c r="G81" t="s">
+        <v>11</v>
+      </c>
+      <c r="H81" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="s">
+        <v>49</v>
+      </c>
+      <c r="B82" t="s">
+        <v>49</v>
+      </c>
+      <c r="C82" t="s">
+        <v>9</v>
+      </c>
+      <c r="D82" t="s">
+        <v>9</v>
+      </c>
+      <c r="E82" t="s">
+        <v>43</v>
+      </c>
+      <c r="F82" t="s">
+        <v>43</v>
+      </c>
+      <c r="G82" t="s">
+        <v>11</v>
+      </c>
+      <c r="H82" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="s">
+        <v>49</v>
+      </c>
+      <c r="B83" t="s">
+        <v>49</v>
+      </c>
+      <c r="C83" t="s">
+        <v>9</v>
+      </c>
+      <c r="D83" t="s">
+        <v>9</v>
+      </c>
+      <c r="E83" t="s">
+        <v>35</v>
+      </c>
+      <c r="F83" t="s">
+        <v>35</v>
+      </c>
+      <c r="G83" t="s">
+        <v>11</v>
+      </c>
+      <c r="H83" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="s">
+        <v>49</v>
+      </c>
+      <c r="B84" t="s">
+        <v>49</v>
+      </c>
+      <c r="C84" t="s">
+        <v>9</v>
+      </c>
+      <c r="D84" t="s">
+        <v>9</v>
+      </c>
+      <c r="E84" t="s">
+        <v>13</v>
+      </c>
+      <c r="F84" t="s">
+        <v>13</v>
+      </c>
+      <c r="G84" t="s">
+        <v>11</v>
+      </c>
+      <c r="H84" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
+        <v>49</v>
+      </c>
+      <c r="B85" t="s">
+        <v>49</v>
+      </c>
+      <c r="C85" t="s">
+        <v>9</v>
+      </c>
+      <c r="D85" t="s">
+        <v>9</v>
+      </c>
+      <c r="E85" t="s">
+        <v>10</v>
+      </c>
+      <c r="F85" t="s">
+        <v>10</v>
+      </c>
+      <c r="G85" t="s">
+        <v>11</v>
+      </c>
+      <c r="H85" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>50</v>
+      </c>
+      <c r="B86" t="s">
+        <v>50</v>
+      </c>
+      <c r="C86" t="s">
+        <v>9</v>
+      </c>
+      <c r="D86" t="s">
+        <v>9</v>
+      </c>
+      <c r="E86" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86" t="s">
+        <v>10</v>
+      </c>
+      <c r="G86" t="s">
+        <v>11</v>
+      </c>
+      <c r="H86" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
         <v>51</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B87" t="s">
         <v>51</v>
       </c>
-      <c r="C30" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="C87" t="s">
+        <v>9</v>
+      </c>
+      <c r="D87" t="s">
+        <v>9</v>
+      </c>
+      <c r="E87" t="s">
+        <v>10</v>
+      </c>
+      <c r="F87" t="s">
+        <v>10</v>
+      </c>
+      <c r="G87" t="s">
+        <v>11</v>
+      </c>
+      <c r="H87" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
         <v>52</v>
       </c>
-      <c r="F30" t="s">
+      <c r="B88" t="s">
         <v>52</v>
       </c>
-      <c r="G30" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" t="s">
+      <c r="C88" t="s">
+        <v>9</v>
+      </c>
+      <c r="D88" t="s">
+        <v>9</v>
+      </c>
+      <c r="E88" t="s">
+        <v>22</v>
+      </c>
+      <c r="F88" t="s">
+        <v>22</v>
+      </c>
+      <c r="G88" t="s">
+        <v>11</v>
+      </c>
+      <c r="H88" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>52</v>
+      </c>
+      <c r="B89" t="s">
+        <v>52</v>
+      </c>
+      <c r="C89" t="s">
+        <v>9</v>
+      </c>
+      <c r="D89" t="s">
+        <v>9</v>
+      </c>
+      <c r="E89" t="s">
+        <v>23</v>
+      </c>
+      <c r="F89" t="s">
+        <v>23</v>
+      </c>
+      <c r="G89" t="s">
+        <v>11</v>
+      </c>
+      <c r="H89" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>52</v>
+      </c>
+      <c r="B90" t="s">
+        <v>52</v>
+      </c>
+      <c r="C90" t="s">
+        <v>9</v>
+      </c>
+      <c r="D90" t="s">
+        <v>9</v>
+      </c>
+      <c r="E90" t="s">
+        <v>43</v>
+      </c>
+      <c r="F90" t="s">
+        <v>43</v>
+      </c>
+      <c r="G90" t="s">
+        <v>11</v>
+      </c>
+      <c r="H90" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>52</v>
+      </c>
+      <c r="B91" t="s">
+        <v>52</v>
+      </c>
+      <c r="C91" t="s">
+        <v>9</v>
+      </c>
+      <c r="D91" t="s">
+        <v>9</v>
+      </c>
+      <c r="E91" t="s">
+        <v>44</v>
+      </c>
+      <c r="F91" t="s">
+        <v>44</v>
+      </c>
+      <c r="G91" t="s">
+        <v>11</v>
+      </c>
+      <c r="H91" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>52</v>
+      </c>
+      <c r="B92" t="s">
+        <v>52</v>
+      </c>
+      <c r="C92" t="s">
+        <v>9</v>
+      </c>
+      <c r="D92" t="s">
+        <v>9</v>
+      </c>
+      <c r="E92" t="s">
+        <v>13</v>
+      </c>
+      <c r="F92" t="s">
+        <v>13</v>
+      </c>
+      <c r="G92" t="s">
+        <v>11</v>
+      </c>
+      <c r="H92" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="s">
+        <v>52</v>
+      </c>
+      <c r="B93" t="s">
+        <v>52</v>
+      </c>
+      <c r="C93" t="s">
+        <v>9</v>
+      </c>
+      <c r="D93" t="s">
+        <v>9</v>
+      </c>
+      <c r="E93" t="s">
+        <v>14</v>
+      </c>
+      <c r="F93" t="s">
+        <v>14</v>
+      </c>
+      <c r="G93" t="s">
+        <v>11</v>
+      </c>
+      <c r="H93" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="s">
+        <v>52</v>
+      </c>
+      <c r="B94" t="s">
+        <v>52</v>
+      </c>
+      <c r="C94" t="s">
+        <v>9</v>
+      </c>
+      <c r="D94" t="s">
+        <v>9</v>
+      </c>
+      <c r="E94" t="s">
+        <v>15</v>
+      </c>
+      <c r="F94" t="s">
+        <v>15</v>
+      </c>
+      <c r="G94" t="s">
+        <v>11</v>
+      </c>
+      <c r="H94" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="s">
+        <v>52</v>
+      </c>
+      <c r="B95" t="s">
+        <v>52</v>
+      </c>
+      <c r="C95" t="s">
+        <v>9</v>
+      </c>
+      <c r="D95" t="s">
+        <v>9</v>
+      </c>
+      <c r="E95" t="s">
+        <v>16</v>
+      </c>
+      <c r="F95" t="s">
+        <v>16</v>
+      </c>
+      <c r="G95" t="s">
+        <v>11</v>
+      </c>
+      <c r="H95" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="s">
+        <v>52</v>
+      </c>
+      <c r="B96" t="s">
+        <v>52</v>
+      </c>
+      <c r="C96" t="s">
+        <v>9</v>
+      </c>
+      <c r="D96" t="s">
+        <v>9</v>
+      </c>
+      <c r="E96" t="s">
+        <v>17</v>
+      </c>
+      <c r="F96" t="s">
+        <v>17</v>
+      </c>
+      <c r="G96" t="s">
+        <v>11</v>
+      </c>
+      <c r="H96" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="s">
+        <v>52</v>
+      </c>
+      <c r="B97" t="s">
+        <v>52</v>
+      </c>
+      <c r="C97" t="s">
+        <v>9</v>
+      </c>
+      <c r="D97" t="s">
+        <v>9</v>
+      </c>
+      <c r="E97" t="s">
+        <v>18</v>
+      </c>
+      <c r="F97" t="s">
+        <v>18</v>
+      </c>
+      <c r="G97" t="s">
+        <v>11</v>
+      </c>
+      <c r="H97" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="s">
+        <v>52</v>
+      </c>
+      <c r="B98" t="s">
+        <v>52</v>
+      </c>
+      <c r="C98" t="s">
+        <v>9</v>
+      </c>
+      <c r="D98" t="s">
+        <v>9</v>
+      </c>
+      <c r="E98" t="s">
+        <v>45</v>
+      </c>
+      <c r="F98" t="s">
+        <v>45</v>
+      </c>
+      <c r="G98" t="s">
+        <v>11</v>
+      </c>
+      <c r="H98" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="s">
+        <v>52</v>
+      </c>
+      <c r="B99" t="s">
+        <v>52</v>
+      </c>
+      <c r="C99" t="s">
+        <v>9</v>
+      </c>
+      <c r="D99" t="s">
+        <v>9</v>
+      </c>
+      <c r="E99" t="s">
+        <v>10</v>
+      </c>
+      <c r="F99" t="s">
+        <v>10</v>
+      </c>
+      <c r="G99" t="s">
+        <v>11</v>
+      </c>
+      <c r="H99" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="s">
+        <v>53</v>
+      </c>
+      <c r="B100" t="s">
+        <v>53</v>
+      </c>
+      <c r="C100" t="s">
+        <v>9</v>
+      </c>
+      <c r="D100" t="s">
+        <v>9</v>
+      </c>
+      <c r="E100" t="s">
+        <v>10</v>
+      </c>
+      <c r="F100" t="s">
+        <v>10</v>
+      </c>
+      <c r="G100" t="s">
+        <v>11</v>
+      </c>
+      <c r="H100" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>54</v>
+      </c>
+      <c r="B101" t="s">
+        <v>54</v>
+      </c>
+      <c r="C101" t="s">
+        <v>9</v>
+      </c>
+      <c r="D101" t="s">
+        <v>9</v>
+      </c>
+      <c r="E101" t="s">
+        <v>22</v>
+      </c>
+      <c r="F101" t="s">
+        <v>22</v>
+      </c>
+      <c r="G101" t="s">
+        <v>11</v>
+      </c>
+      <c r="H101" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>54</v>
+      </c>
+      <c r="B102" t="s">
+        <v>54</v>
+      </c>
+      <c r="C102" t="s">
+        <v>9</v>
+      </c>
+      <c r="D102" t="s">
+        <v>9</v>
+      </c>
+      <c r="E102" t="s">
+        <v>23</v>
+      </c>
+      <c r="F102" t="s">
+        <v>23</v>
+      </c>
+      <c r="G102" t="s">
+        <v>11</v>
+      </c>
+      <c r="H102" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>54</v>
+      </c>
+      <c r="B103" t="s">
+        <v>54</v>
+      </c>
+      <c r="C103" t="s">
+        <v>9</v>
+      </c>
+      <c r="D103" t="s">
+        <v>9</v>
+      </c>
+      <c r="E103" t="s">
+        <v>35</v>
+      </c>
+      <c r="F103" t="s">
+        <v>35</v>
+      </c>
+      <c r="G103" t="s">
+        <v>11</v>
+      </c>
+      <c r="H103" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>54</v>
+      </c>
+      <c r="B104" t="s">
+        <v>54</v>
+      </c>
+      <c r="C104" t="s">
+        <v>9</v>
+      </c>
+      <c r="D104" t="s">
+        <v>9</v>
+      </c>
+      <c r="E104" t="s">
+        <v>13</v>
+      </c>
+      <c r="F104" t="s">
+        <v>13</v>
+      </c>
+      <c r="G104" t="s">
+        <v>11</v>
+      </c>
+      <c r="H104" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>54</v>
+      </c>
+      <c r="B105" t="s">
+        <v>54</v>
+      </c>
+      <c r="C105" t="s">
+        <v>9</v>
+      </c>
+      <c r="D105" t="s">
+        <v>9</v>
+      </c>
+      <c r="E105" t="s">
+        <v>10</v>
+      </c>
+      <c r="F105" t="s">
+        <v>10</v>
+      </c>
+      <c r="G105" t="s">
+        <v>11</v>
+      </c>
+      <c r="H105" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>55</v>
+      </c>
+      <c r="B106" t="s">
+        <v>55</v>
+      </c>
+      <c r="C106" t="s">
+        <v>9</v>
+      </c>
+      <c r="D106" t="s">
+        <v>9</v>
+      </c>
+      <c r="E106" t="s">
+        <v>22</v>
+      </c>
+      <c r="F106" t="s">
+        <v>22</v>
+      </c>
+      <c r="G106" t="s">
+        <v>11</v>
+      </c>
+      <c r="H106" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>55</v>
+      </c>
+      <c r="B107" t="s">
+        <v>55</v>
+      </c>
+      <c r="C107" t="s">
+        <v>9</v>
+      </c>
+      <c r="D107" t="s">
+        <v>9</v>
+      </c>
+      <c r="E107" t="s">
+        <v>23</v>
+      </c>
+      <c r="F107" t="s">
+        <v>23</v>
+      </c>
+      <c r="G107" t="s">
+        <v>11</v>
+      </c>
+      <c r="H107" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>55</v>
+      </c>
+      <c r="B108" t="s">
+        <v>55</v>
+      </c>
+      <c r="C108" t="s">
+        <v>9</v>
+      </c>
+      <c r="D108" t="s">
+        <v>9</v>
+      </c>
+      <c r="E108" t="s">
+        <v>43</v>
+      </c>
+      <c r="F108" t="s">
+        <v>43</v>
+      </c>
+      <c r="G108" t="s">
+        <v>11</v>
+      </c>
+      <c r="H108" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>55</v>
+      </c>
+      <c r="B109" t="s">
+        <v>55</v>
+      </c>
+      <c r="C109" t="s">
+        <v>9</v>
+      </c>
+      <c r="D109" t="s">
+        <v>9</v>
+      </c>
+      <c r="E109" t="s">
+        <v>44</v>
+      </c>
+      <c r="F109" t="s">
+        <v>44</v>
+      </c>
+      <c r="G109" t="s">
+        <v>11</v>
+      </c>
+      <c r="H109" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>55</v>
+      </c>
+      <c r="B110" t="s">
+        <v>55</v>
+      </c>
+      <c r="C110" t="s">
+        <v>9</v>
+      </c>
+      <c r="D110" t="s">
+        <v>9</v>
+      </c>
+      <c r="E110" t="s">
+        <v>13</v>
+      </c>
+      <c r="F110" t="s">
+        <v>13</v>
+      </c>
+      <c r="G110" t="s">
+        <v>11</v>
+      </c>
+      <c r="H110" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>55</v>
+      </c>
+      <c r="B111" t="s">
+        <v>55</v>
+      </c>
+      <c r="C111" t="s">
+        <v>9</v>
+      </c>
+      <c r="D111" t="s">
+        <v>9</v>
+      </c>
+      <c r="E111" t="s">
+        <v>14</v>
+      </c>
+      <c r="F111" t="s">
+        <v>14</v>
+      </c>
+      <c r="G111" t="s">
+        <v>11</v>
+      </c>
+      <c r="H111" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>55</v>
+      </c>
+      <c r="B112" t="s">
+        <v>55</v>
+      </c>
+      <c r="C112" t="s">
+        <v>9</v>
+      </c>
+      <c r="D112" t="s">
+        <v>9</v>
+      </c>
+      <c r="E112" t="s">
+        <v>15</v>
+      </c>
+      <c r="F112" t="s">
+        <v>15</v>
+      </c>
+      <c r="G112" t="s">
+        <v>11</v>
+      </c>
+      <c r="H112" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>55</v>
+      </c>
+      <c r="B113" t="s">
+        <v>55</v>
+      </c>
+      <c r="C113" t="s">
+        <v>9</v>
+      </c>
+      <c r="D113" t="s">
+        <v>9</v>
+      </c>
+      <c r="E113" t="s">
+        <v>16</v>
+      </c>
+      <c r="F113" t="s">
+        <v>16</v>
+      </c>
+      <c r="G113" t="s">
+        <v>11</v>
+      </c>
+      <c r="H113" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>55</v>
+      </c>
+      <c r="B114" t="s">
+        <v>55</v>
+      </c>
+      <c r="C114" t="s">
+        <v>9</v>
+      </c>
+      <c r="D114" t="s">
+        <v>9</v>
+      </c>
+      <c r="E114" t="s">
+        <v>10</v>
+      </c>
+      <c r="F114" t="s">
+        <v>10</v>
+      </c>
+      <c r="G114" t="s">
+        <v>11</v>
+      </c>
+      <c r="H114" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>56</v>
+      </c>
+      <c r="B115" t="s">
+        <v>56</v>
+      </c>
+      <c r="C115" t="s">
+        <v>9</v>
+      </c>
+      <c r="D115" t="s">
+        <v>9</v>
+      </c>
+      <c r="E115" t="s">
+        <v>22</v>
+      </c>
+      <c r="F115" t="s">
+        <v>22</v>
+      </c>
+      <c r="G115" t="s">
+        <v>11</v>
+      </c>
+      <c r="H115" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>56</v>
+      </c>
+      <c r="B116" t="s">
+        <v>56</v>
+      </c>
+      <c r="C116" t="s">
+        <v>9</v>
+      </c>
+      <c r="D116" t="s">
+        <v>9</v>
+      </c>
+      <c r="E116" t="s">
+        <v>23</v>
+      </c>
+      <c r="F116" t="s">
+        <v>23</v>
+      </c>
+      <c r="G116" t="s">
+        <v>11</v>
+      </c>
+      <c r="H116" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="s">
+        <v>56</v>
+      </c>
+      <c r="B117" t="s">
+        <v>56</v>
+      </c>
+      <c r="C117" t="s">
+        <v>9</v>
+      </c>
+      <c r="D117" t="s">
+        <v>9</v>
+      </c>
+      <c r="E117" t="s">
+        <v>43</v>
+      </c>
+      <c r="F117" t="s">
+        <v>43</v>
+      </c>
+      <c r="G117" t="s">
+        <v>11</v>
+      </c>
+      <c r="H117" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="s">
+        <v>56</v>
+      </c>
+      <c r="B118" t="s">
+        <v>56</v>
+      </c>
+      <c r="C118" t="s">
+        <v>9</v>
+      </c>
+      <c r="D118" t="s">
+        <v>9</v>
+      </c>
+      <c r="E118" t="s">
+        <v>44</v>
+      </c>
+      <c r="F118" t="s">
+        <v>44</v>
+      </c>
+      <c r="G118" t="s">
+        <v>11</v>
+      </c>
+      <c r="H118" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="s">
+        <v>56</v>
+      </c>
+      <c r="B119" t="s">
+        <v>56</v>
+      </c>
+      <c r="C119" t="s">
+        <v>9</v>
+      </c>
+      <c r="D119" t="s">
+        <v>9</v>
+      </c>
+      <c r="E119" t="s">
+        <v>35</v>
+      </c>
+      <c r="F119" t="s">
+        <v>35</v>
+      </c>
+      <c r="G119" t="s">
+        <v>11</v>
+      </c>
+      <c r="H119" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="s">
+        <v>56</v>
+      </c>
+      <c r="B120" t="s">
+        <v>56</v>
+      </c>
+      <c r="C120" t="s">
+        <v>9</v>
+      </c>
+      <c r="D120" t="s">
+        <v>9</v>
+      </c>
+      <c r="E120" t="s">
+        <v>13</v>
+      </c>
+      <c r="F120" t="s">
+        <v>13</v>
+      </c>
+      <c r="G120" t="s">
+        <v>11</v>
+      </c>
+      <c r="H120" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="s">
+        <v>56</v>
+      </c>
+      <c r="B121" t="s">
+        <v>56</v>
+      </c>
+      <c r="C121" t="s">
+        <v>9</v>
+      </c>
+      <c r="D121" t="s">
+        <v>9</v>
+      </c>
+      <c r="E121" t="s">
+        <v>10</v>
+      </c>
+      <c r="F121" t="s">
+        <v>10</v>
+      </c>
+      <c r="G121" t="s">
+        <v>11</v>
+      </c>
+      <c r="H121" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="s">
+        <v>57</v>
+      </c>
+      <c r="B122" t="s">
+        <v>57</v>
+      </c>
+      <c r="C122" t="s">
+        <v>9</v>
+      </c>
+      <c r="D122" t="s">
+        <v>9</v>
+      </c>
+      <c r="E122" t="s">
+        <v>10</v>
+      </c>
+      <c r="F122" t="s">
+        <v>10</v>
+      </c>
+      <c r="G122" t="s">
+        <v>11</v>
+      </c>
+      <c r="H122" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="s">
+        <v>58</v>
+      </c>
+      <c r="B123" t="s">
+        <v>58</v>
+      </c>
+      <c r="C123" t="s">
+        <v>9</v>
+      </c>
+      <c r="D123" t="s">
+        <v>9</v>
+      </c>
+      <c r="E123" t="s">
+        <v>10</v>
+      </c>
+      <c r="F123" t="s">
+        <v>10</v>
+      </c>
+      <c r="G123" t="s">
+        <v>11</v>
+      </c>
+      <c r="H123" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="s">
+        <v>59</v>
+      </c>
+      <c r="B124" t="s">
+        <v>59</v>
+      </c>
+      <c r="C124" t="s">
+        <v>9</v>
+      </c>
+      <c r="D124" t="s">
+        <v>9</v>
+      </c>
+      <c r="E124" t="s">
+        <v>10</v>
+      </c>
+      <c r="F124" t="s">
+        <v>10</v>
+      </c>
+      <c r="G124" t="s">
+        <v>11</v>
+      </c>
+      <c r="H124" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="s">
+        <v>60</v>
+      </c>
+      <c r="B125" t="s">
+        <v>60</v>
+      </c>
+      <c r="C125" t="s">
+        <v>9</v>
+      </c>
+      <c r="D125" t="s">
+        <v>9</v>
+      </c>
+      <c r="E125" t="s">
+        <v>10</v>
+      </c>
+      <c r="F125" t="s">
+        <v>10</v>
+      </c>
+      <c r="G125" t="s">
+        <v>11</v>
+      </c>
+      <c r="H125" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>61</v>
+      </c>
+      <c r="B126" t="s">
+        <v>61</v>
+      </c>
+      <c r="C126" t="s">
+        <v>9</v>
+      </c>
+      <c r="D126" t="s">
+        <v>9</v>
+      </c>
+      <c r="E126" t="s">
+        <v>22</v>
+      </c>
+      <c r="F126" t="s">
+        <v>22</v>
+      </c>
+      <c r="G126" t="s">
+        <v>11</v>
+      </c>
+      <c r="H126" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>61</v>
+      </c>
+      <c r="B127" t="s">
+        <v>61</v>
+      </c>
+      <c r="C127" t="s">
+        <v>9</v>
+      </c>
+      <c r="D127" t="s">
+        <v>9</v>
+      </c>
+      <c r="E127" t="s">
+        <v>23</v>
+      </c>
+      <c r="F127" t="s">
+        <v>23</v>
+      </c>
+      <c r="G127" t="s">
+        <v>11</v>
+      </c>
+      <c r="H127" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>61</v>
+      </c>
+      <c r="B128" t="s">
+        <v>61</v>
+      </c>
+      <c r="C128" t="s">
+        <v>9</v>
+      </c>
+      <c r="D128" t="s">
+        <v>9</v>
+      </c>
+      <c r="E128" t="s">
+        <v>35</v>
+      </c>
+      <c r="F128" t="s">
+        <v>35</v>
+      </c>
+      <c r="G128" t="s">
+        <v>11</v>
+      </c>
+      <c r="H128" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>61</v>
+      </c>
+      <c r="B129" t="s">
+        <v>61</v>
+      </c>
+      <c r="C129" t="s">
+        <v>9</v>
+      </c>
+      <c r="D129" t="s">
+        <v>9</v>
+      </c>
+      <c r="E129" t="s">
+        <v>13</v>
+      </c>
+      <c r="F129" t="s">
+        <v>13</v>
+      </c>
+      <c r="G129" t="s">
+        <v>11</v>
+      </c>
+      <c r="H129" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>61</v>
+      </c>
+      <c r="B130" t="s">
+        <v>61</v>
+      </c>
+      <c r="C130" t="s">
+        <v>9</v>
+      </c>
+      <c r="D130" t="s">
+        <v>9</v>
+      </c>
+      <c r="E130" t="s">
+        <v>14</v>
+      </c>
+      <c r="F130" t="s">
+        <v>14</v>
+      </c>
+      <c r="G130" t="s">
+        <v>11</v>
+      </c>
+      <c r="H130" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>61</v>
+      </c>
+      <c r="B131" t="s">
+        <v>61</v>
+      </c>
+      <c r="C131" t="s">
+        <v>9</v>
+      </c>
+      <c r="D131" t="s">
+        <v>9</v>
+      </c>
+      <c r="E131" t="s">
+        <v>15</v>
+      </c>
+      <c r="F131" t="s">
+        <v>15</v>
+      </c>
+      <c r="G131" t="s">
+        <v>11</v>
+      </c>
+      <c r="H131" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>61</v>
+      </c>
+      <c r="B132" t="s">
+        <v>61</v>
+      </c>
+      <c r="C132" t="s">
+        <v>9</v>
+      </c>
+      <c r="D132" t="s">
+        <v>9</v>
+      </c>
+      <c r="E132" t="s">
+        <v>16</v>
+      </c>
+      <c r="F132" t="s">
+        <v>16</v>
+      </c>
+      <c r="G132" t="s">
+        <v>11</v>
+      </c>
+      <c r="H132" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>61</v>
+      </c>
+      <c r="B133" t="s">
+        <v>61</v>
+      </c>
+      <c r="C133" t="s">
+        <v>9</v>
+      </c>
+      <c r="D133" t="s">
+        <v>9</v>
+      </c>
+      <c r="E133" t="s">
+        <v>17</v>
+      </c>
+      <c r="F133" t="s">
+        <v>17</v>
+      </c>
+      <c r="G133" t="s">
+        <v>11</v>
+      </c>
+      <c r="H133" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>61</v>
+      </c>
+      <c r="B134" t="s">
+        <v>61</v>
+      </c>
+      <c r="C134" t="s">
+        <v>9</v>
+      </c>
+      <c r="D134" t="s">
+        <v>9</v>
+      </c>
+      <c r="E134" t="s">
+        <v>45</v>
+      </c>
+      <c r="F134" t="s">
+        <v>45</v>
+      </c>
+      <c r="G134" t="s">
+        <v>11</v>
+      </c>
+      <c r="H134" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>61</v>
+      </c>
+      <c r="B135" t="s">
+        <v>61</v>
+      </c>
+      <c r="C135" t="s">
+        <v>9</v>
+      </c>
+      <c r="D135" t="s">
+        <v>9</v>
+      </c>
+      <c r="E135" t="s">
+        <v>10</v>
+      </c>
+      <c r="F135" t="s">
+        <v>10</v>
+      </c>
+      <c r="G135" t="s">
+        <v>11</v>
+      </c>
+      <c r="H135" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>62</v>
+      </c>
+      <c r="B136" t="s">
+        <v>62</v>
+      </c>
+      <c r="C136" t="s">
+        <v>9</v>
+      </c>
+      <c r="D136" t="s">
+        <v>9</v>
+      </c>
+      <c r="E136" t="s">
+        <v>22</v>
+      </c>
+      <c r="F136" t="s">
+        <v>22</v>
+      </c>
+      <c r="G136" t="s">
+        <v>11</v>
+      </c>
+      <c r="H136" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
+        <v>62</v>
+      </c>
+      <c r="B137" t="s">
+        <v>62</v>
+      </c>
+      <c r="C137" t="s">
+        <v>9</v>
+      </c>
+      <c r="D137" t="s">
+        <v>9</v>
+      </c>
+      <c r="E137" t="s">
+        <v>35</v>
+      </c>
+      <c r="F137" t="s">
+        <v>35</v>
+      </c>
+      <c r="G137" t="s">
+        <v>11</v>
+      </c>
+      <c r="H137" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="s">
+        <v>62</v>
+      </c>
+      <c r="B138" t="s">
+        <v>62</v>
+      </c>
+      <c r="C138" t="s">
+        <v>9</v>
+      </c>
+      <c r="D138" t="s">
+        <v>9</v>
+      </c>
+      <c r="E138" t="s">
+        <v>13</v>
+      </c>
+      <c r="F138" t="s">
+        <v>13</v>
+      </c>
+      <c r="G138" t="s">
+        <v>11</v>
+      </c>
+      <c r="H138" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="s">
+        <v>62</v>
+      </c>
+      <c r="B139" t="s">
+        <v>62</v>
+      </c>
+      <c r="C139" t="s">
+        <v>9</v>
+      </c>
+      <c r="D139" t="s">
+        <v>9</v>
+      </c>
+      <c r="E139" t="s">
+        <v>24</v>
+      </c>
+      <c r="F139" t="s">
+        <v>24</v>
+      </c>
+      <c r="G139" t="s">
+        <v>11</v>
+      </c>
+      <c r="H139" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="s">
+        <v>62</v>
+      </c>
+      <c r="B140" t="s">
+        <v>62</v>
+      </c>
+      <c r="C140" t="s">
+        <v>9</v>
+      </c>
+      <c r="D140" t="s">
+        <v>9</v>
+      </c>
+      <c r="E140" t="s">
+        <v>10</v>
+      </c>
+      <c r="F140" t="s">
+        <v>10</v>
+      </c>
+      <c r="G140" t="s">
+        <v>11</v>
+      </c>
+      <c r="H140" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1336,7 +4226,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2">
@@ -1357,218 +4247,218 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>